<commit_message>
Boosted Tree Model Working fine
Warning due to CUDA toolkit and cuDNN installation.
</commit_message>
<xml_diff>
--- a/Observation.xlsx
+++ b/Observation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Application of Boosted Tree Classifier for Predicting Disease from Symptoms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Application-of-Boosted-Tree-Classifier-for-Predicting-Disease-from-Symptoms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC560D1-8642-4373-AAFE-54A564F927F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC644BAD-687A-4EAC-8506-3EAB32E2E58D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
   <si>
     <t>Learning Rate</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Accuracy</t>
+  </si>
+  <si>
+    <t>No. of batches per layer</t>
+  </si>
+  <si>
+    <t>Average Loss</t>
+  </si>
+  <si>
+    <t>Loss</t>
   </si>
 </sst>
 </file>
@@ -375,23 +384,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="19.5546875" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30.5546875" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,12 +414,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -419,10 +440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E254EF9D-26E4-4AF8-872E-1C6A354B39CB}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,11 +451,14 @@
     <col min="1" max="2" width="17.77734375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,12 +469,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -461,10 +494,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0C78ED-BD76-4EA0-85CF-3439E966A149}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,11 +506,14 @@
     <col min="2" max="2" width="17.77734375" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,12 +524,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -504,10 +549,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E78E705-DC29-4E6D-98FF-DA0035A5F8E6}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,11 +560,14 @@
     <col min="1" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.109375" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,12 +578,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>